<commit_message>
Update src process to JSON/CSV/PDF
</commit_message>
<xml_diff>
--- a/Learning GIT command.xlsx
+++ b/Learning GIT command.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>https://help.github.com/articles/adding-an-existing-project-to-github-using-the-command-line/</t>
   </si>
@@ -116,6 +116,18 @@
   </si>
   <si>
     <t>Add toàn bộ files/folder có trong folder lên Git branch</t>
+  </si>
+  <si>
+    <t>#8</t>
+  </si>
+  <si>
+    <t>Add thêm 1 file bất kì nào đó sau khi đã add done toàn bộ folder.</t>
+  </si>
+  <si>
+    <t>git commit -m "Add guidline Excel file"</t>
+  </si>
+  <si>
+    <t>Add thêm 2 file guilde lên branch</t>
   </si>
 </sst>
 </file>
@@ -211,14 +223,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,6 +934,53 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>271</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>289</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="347382" y="52129765"/>
+          <a:ext cx="5777193" cy="3600450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1210,10 +1269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE270"/>
+  <dimension ref="A1:AE294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AK230" sqref="AK230"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AE274" sqref="AE274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="15"/>
@@ -1222,15 +1281,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="7">
+      <c r="A1" s="8">
         <v>43332</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:19" ht="21">
       <c r="A2" s="5" t="s">
@@ -1276,7 +1335,7 @@
       </c>
     </row>
     <row r="69" spans="1:2" ht="18.75">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -1284,7 +1343,7 @@
       </c>
     </row>
     <row r="87" spans="1:2" ht="18.75">
-      <c r="A87" s="9" t="s">
+      <c r="A87" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -1292,7 +1351,7 @@
       </c>
     </row>
     <row r="129" spans="1:2" ht="18.75">
-      <c r="A129" s="9" t="s">
+      <c r="A129" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B129" s="1" t="s">
@@ -1300,7 +1359,7 @@
       </c>
     </row>
     <row r="158" spans="1:2" ht="18.75">
-      <c r="A158" s="9" t="s">
+      <c r="A158" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B158" s="1" t="s">
@@ -1433,7 +1492,7 @@
       <c r="B199" s="3"/>
     </row>
     <row r="200" spans="1:2" ht="18.75">
-      <c r="A200" s="9" t="s">
+      <c r="A200" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B200" s="1" t="s">
@@ -1479,7 +1538,7 @@
       <c r="B212" s="3"/>
     </row>
     <row r="213" spans="1:2" ht="18.75">
-      <c r="A213" s="9" t="s">
+      <c r="A213" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B213" s="1" t="s">
@@ -1487,7 +1546,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" ht="18.75">
-      <c r="A223" s="9" t="s">
+      <c r="A223" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B223" s="1" t="s">
@@ -1551,8 +1610,60 @@
         <v>27</v>
       </c>
     </row>
-    <row r="270" spans="1:31" ht="21">
-      <c r="A270" s="5" t="s">
+    <row r="271" spans="1:31" ht="18.75">
+      <c r="A271" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="273" spans="30:31">
+      <c r="AD273" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE273" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="30:31">
+      <c r="AE274" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="278" spans="30:31">
+      <c r="AD278" s="6">
+        <v>2</v>
+      </c>
+      <c r="AE278" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="279" spans="30:31">
+      <c r="AE279" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="30:31">
+      <c r="AD281" s="6">
+        <v>3</v>
+      </c>
+      <c r="AE281" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="282" spans="30:31">
+      <c r="AE282" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="283" spans="30:31">
+      <c r="AD283" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" ht="21">
+      <c r="A294" s="5" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>